<commit_message>
Graphs For Lab 5
Yeah we forgot to ever make this
</commit_message>
<xml_diff>
--- a/Lab 6/Data/Run_1.xlsx
+++ b/Lab 6/Data/Run_1.xlsx
@@ -1048,11 +1048,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89733376"/>
-        <c:axId val="89739648"/>
+        <c:axId val="98580736"/>
+        <c:axId val="98587008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89733376"/>
+        <c:axId val="98580736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,12 +1081,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89739648"/>
+        <c:crossAx val="98587008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89739648"/>
+        <c:axId val="98587008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1117,7 +1117,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89733376"/>
+        <c:crossAx val="98580736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>